<commit_message>
New Update with proper case study ppt
</commit_message>
<xml_diff>
--- a/Controller.xlsx
+++ b/Controller.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="112">
   <si>
     <t>Browser</t>
   </si>
@@ -157,218 +157,209 @@
     <t>Present Status</t>
   </si>
   <si>
-    <t>Abhijit.Das@cit.com</t>
+    <t>/^(?=[^.])[a-zA-Z0-9.\-_]*[a-zA-Z0-9\-_]@[a-zA-Z0-9]+(\.[a-zA-Z]{2,})+$/</t>
+  </si>
+  <si>
+    <t>Reporting Mode</t>
+  </si>
+  <si>
+    <t>Attachment</t>
+  </si>
+  <si>
+    <t>Mail</t>
+  </si>
+  <si>
+    <t>SharePoint</t>
+  </si>
+  <si>
+    <t>Both</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>Executive Summary Report</t>
+  </si>
+  <si>
+    <t>Zip Report (Summary + Individual Test Case Report)</t>
+  </si>
+  <si>
+    <t>Note: Available Reporting modes</t>
+  </si>
+  <si>
+    <t>Note: Available Attachments</t>
+  </si>
+  <si>
+    <t>Sharepoint Link</t>
+  </si>
+  <si>
+    <t>Email_Invalid3</t>
+  </si>
+  <si>
+    <t>Email_Invalid4</t>
+  </si>
+  <si>
+    <t>Email_Invalid5</t>
+  </si>
+  <si>
+    <t>Email_Invalid6</t>
+  </si>
+  <si>
+    <t>Email_Invalid7</t>
+  </si>
+  <si>
+    <t>Email_Invalid8</t>
+  </si>
+  <si>
+    <t>Abc.example.com</t>
+  </si>
+  <si>
+    <t>A@b@c@example.com</t>
+  </si>
+  <si>
+    <t>no @ character</t>
+  </si>
+  <si>
+    <t>only one @ is allowed outside quotation marks</t>
+  </si>
+  <si>
+    <t>a"b(c)d,e:f;g&lt;h&gt;i[j\k]l@example.com</t>
+  </si>
+  <si>
+    <t>none of the special characters in this local-part are allowed outside quotation marks</t>
+  </si>
+  <si>
+    <t>just"not"right@example.com</t>
+  </si>
+  <si>
+    <t>quoted strings must be dot separated or the only element making up the local-part</t>
+  </si>
+  <si>
+    <t>this is"not\allowed@example.com</t>
+  </si>
+  <si>
+    <t>spaces, quotes, and backslashes may only exist when within quoted strings and preceded by a backslash</t>
+  </si>
+  <si>
+    <t>this\ still\"not\\allowed@example.com</t>
+  </si>
+  <si>
+    <t>even if escaped (preceded by a backslash), spaces, quotes, and backslashes must still be contained by quotes</t>
+  </si>
+  <si>
+    <t>john..doe@example.com</t>
+  </si>
+  <si>
+    <t>(double dot before @</t>
+  </si>
+  <si>
+    <t>Email_Invalid9</t>
+  </si>
+  <si>
+    <t>example@localhost</t>
+  </si>
+  <si>
+    <t>sent from localhost</t>
+  </si>
+  <si>
+    <t>john.doe@example..com</t>
+  </si>
+  <si>
+    <t>double dot after @</t>
+  </si>
+  <si>
+    <t>Info</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>IE</t>
+  </si>
+  <si>
+    <t>QA_1</t>
+  </si>
+  <si>
+    <t>QA_2</t>
+  </si>
+  <si>
+    <t>QA_3</t>
+  </si>
+  <si>
+    <t>QA_4</t>
+  </si>
+  <si>
+    <t>QA_5</t>
+  </si>
+  <si>
+    <t>QA_6</t>
+  </si>
+  <si>
+    <t>QA_7</t>
+  </si>
+  <si>
+    <t>QA_8</t>
+  </si>
+  <si>
+    <t>QA_9</t>
+  </si>
+  <si>
+    <t>QA_10</t>
+  </si>
+  <si>
+    <t>QA_13</t>
+  </si>
+  <si>
+    <t>QA_14</t>
+  </si>
+  <si>
+    <t>QA_15</t>
+  </si>
+  <si>
+    <t>QA_16</t>
+  </si>
+  <si>
+    <t>QA_17</t>
+  </si>
+  <si>
+    <t>QA_18</t>
+  </si>
+  <si>
+    <t>QA_19</t>
+  </si>
+  <si>
+    <t>QA_20</t>
+  </si>
+  <si>
+    <t>QA_21</t>
+  </si>
+  <si>
+    <t>QA_22</t>
+  </si>
+  <si>
+    <t>C:\Dev\Automation Test Base Framework(UFT12.02 + HTML + VB Script)\DemoSharePointLocation</t>
+  </si>
+  <si>
+    <t>http://newtours.demoaut.com/index.php</t>
   </si>
   <si>
     <t>PASS</t>
   </si>
   <si>
-    <t>/^(?=[^.])[a-zA-Z0-9.\-_]*[a-zA-Z0-9\-_]@[a-zA-Z0-9]+(\.[a-zA-Z]{2,})+$/</t>
-  </si>
-  <si>
-    <t>Reporting Mode</t>
-  </si>
-  <si>
-    <t>Attachment</t>
-  </si>
-  <si>
-    <t>Mail</t>
-  </si>
-  <si>
-    <t>SharePoint</t>
-  </si>
-  <si>
-    <t>Both</t>
-  </si>
-  <si>
-    <t>None</t>
-  </si>
-  <si>
-    <t>Executive Summary Report</t>
-  </si>
-  <si>
-    <t>Zip Report (Summary + Individual Test Case Report)</t>
-  </si>
-  <si>
-    <t>Note: Available Reporting modes</t>
-  </si>
-  <si>
-    <t>Note: Available Attachments</t>
-  </si>
-  <si>
-    <t>Sharepoint Link</t>
-  </si>
-  <si>
-    <t>QDSMP1_Service Requests_View Request Asset Location Change Modal</t>
-  </si>
-  <si>
-    <t>QDSMP1_Service Requests_Click x to close</t>
-  </si>
-  <si>
-    <t>QDSMP1_Service Requests_Click Comment field</t>
-  </si>
-  <si>
-    <t>QDSMP1_Service Requests_Click Cancel button</t>
-  </si>
-  <si>
-    <t>QDSMP1_Service Requests_Submit button</t>
-  </si>
-  <si>
-    <t>QDSMP1_Service Requests_Click option in Whats the best way to contact you drop down</t>
-  </si>
-  <si>
-    <t>QDSMP1_Service Requests_Click Best Contact Information field</t>
-  </si>
-  <si>
-    <t>QDSMP1_Service Requests_Inactive Submit Button</t>
-  </si>
-  <si>
-    <t>QDSMP1_Service Requests_Submit Successful Message When Click Submit and Request</t>
-  </si>
-  <si>
-    <t>QDSMP1_Service Requests_Click Close Button</t>
-  </si>
-  <si>
-    <t>QDSMP1_Service Requests_Create Request Asset Location Change</t>
-  </si>
-  <si>
-    <t>QDSMP1_Assets_View Lease Details Page - Assets Tab</t>
-  </si>
-  <si>
-    <t>QDSMP1_Assets_View Assets page at CCAN Level</t>
-  </si>
-  <si>
-    <t>QDSMP1_Assets_View Assets page at Contract Level</t>
-  </si>
-  <si>
-    <t>QDSMP1_Assets_View Asset List - CCAN Level</t>
-  </si>
-  <si>
-    <t>QDSMP1_Assets_View Asset List - Contract Level</t>
-  </si>
-  <si>
-    <t>QDSMP1_Assets_Download CSV</t>
-  </si>
-  <si>
-    <t>QDSMP1_Assets_Pagination</t>
-  </si>
-  <si>
-    <t>Email_Invalid3</t>
-  </si>
-  <si>
-    <t>Email_Invalid4</t>
-  </si>
-  <si>
-    <t>Email_Invalid5</t>
-  </si>
-  <si>
-    <t>Email_Invalid6</t>
-  </si>
-  <si>
-    <t>Email_Invalid7</t>
-  </si>
-  <si>
-    <t>Email_Invalid8</t>
-  </si>
-  <si>
-    <t>Abc.example.com</t>
-  </si>
-  <si>
-    <t>A@b@c@example.com</t>
-  </si>
-  <si>
-    <t>no @ character</t>
-  </si>
-  <si>
-    <t>only one @ is allowed outside quotation marks</t>
-  </si>
-  <si>
-    <t>a"b(c)d,e:f;g&lt;h&gt;i[j\k]l@example.com</t>
-  </si>
-  <si>
-    <t>none of the special characters in this local-part are allowed outside quotation marks</t>
-  </si>
-  <si>
-    <t>just"not"right@example.com</t>
-  </si>
-  <si>
-    <t>quoted strings must be dot separated or the only element making up the local-part</t>
-  </si>
-  <si>
-    <t>this is"not\allowed@example.com</t>
-  </si>
-  <si>
-    <t>spaces, quotes, and backslashes may only exist when within quoted strings and preceded by a backslash</t>
-  </si>
-  <si>
-    <t>this\ still\"not\\allowed@example.com</t>
-  </si>
-  <si>
-    <t>even if escaped (preceded by a backslash), spaces, quotes, and backslashes must still be contained by quotes</t>
-  </si>
-  <si>
-    <t>john..doe@example.com</t>
-  </si>
-  <si>
-    <t>(double dot before @</t>
-  </si>
-  <si>
-    <t>Email_Invalid9</t>
-  </si>
-  <si>
-    <t>example@localhost</t>
-  </si>
-  <si>
-    <t>sent from localhost</t>
-  </si>
-  <si>
-    <t>john.doe@example..com</t>
-  </si>
-  <si>
-    <t>double dot after @</t>
-  </si>
-  <si>
-    <t>Info</t>
-  </si>
-  <si>
-    <t>FAIL</t>
-  </si>
-  <si>
-    <t>QDSMP2_CrossSellFlag_View Dashboard - SOL = Y</t>
-  </si>
-  <si>
-    <t>QDSMP2_CrossSellFlag_View Dashboard - SOL = N or Null</t>
-  </si>
-  <si>
-    <t>QDSMP2_CrossSellFlag_Multiple CCANs on one customer profile</t>
-  </si>
-  <si>
-    <t>QDSMP2_CrossSellFlag_Multiple Contracts on one CCAN</t>
-  </si>
-  <si>
-    <t>Change Data File every day</t>
-  </si>
-  <si>
-    <t>No</t>
-  </si>
-  <si>
-    <t>Sunil.Panjiara@cit.com</t>
-  </si>
-  <si>
-    <t>https://customer.directcapital-sit.com/</t>
-  </si>
-  <si>
-    <t>\\citnet.cit.com\livfile\STS_VF_eComm\Portal\Testing\Internal_Email_Invoicing_DEV</t>
-  </si>
-  <si>
-    <t>https://customer.directcapital-test2.com/</t>
+    <t>QA_11</t>
+  </si>
+  <si>
+    <t>QA_12</t>
+  </si>
+  <si>
+    <t>Abhijit.Das@test.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -408,14 +399,6 @@
       <color rgb="FF222222"/>
       <name val="Arial"/>
       <family val="2"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="4">
@@ -499,17 +482,15 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -547,12 +528,8 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -856,7 +833,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D7" sqref="D7"/>
+      <selection pane="bottomLeft" activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -902,16 +879,16 @@
         <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>60</v>
+        <v>86</v>
       </c>
       <c r="D2" t="s">
-        <v>110</v>
+        <v>6</v>
       </c>
       <c r="E2" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="F2" t="s">
-        <v>47</v>
+        <v>108</v>
       </c>
       <c r="G2" t="s">
         <v>14</v>
@@ -925,16 +902,10 @@
         <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>61</v>
+        <v>87</v>
       </c>
       <c r="D3" t="s">
-        <v>110</v>
-      </c>
-      <c r="E3" t="s">
-        <v>47</v>
-      </c>
-      <c r="F3" t="s">
-        <v>47</v>
+        <v>84</v>
       </c>
       <c r="G3" t="s">
         <v>14</v>
@@ -948,16 +919,10 @@
         <v>7</v>
       </c>
       <c r="C4" t="s">
-        <v>63</v>
+        <v>88</v>
       </c>
       <c r="D4" t="s">
-        <v>110</v>
-      </c>
-      <c r="E4" t="s">
-        <v>47</v>
-      </c>
-      <c r="F4" t="s">
-        <v>47</v>
+        <v>84</v>
       </c>
       <c r="G4" t="s">
         <v>14</v>
@@ -971,16 +936,10 @@
         <v>7</v>
       </c>
       <c r="C5" t="s">
-        <v>62</v>
+        <v>89</v>
       </c>
       <c r="D5" t="s">
-        <v>110</v>
-      </c>
-      <c r="E5" t="s">
-        <v>104</v>
-      </c>
-      <c r="F5" t="s">
-        <v>47</v>
+        <v>84</v>
       </c>
       <c r="G5" t="s">
         <v>14</v>
@@ -994,16 +953,10 @@
         <v>7</v>
       </c>
       <c r="C6" t="s">
-        <v>64</v>
+        <v>90</v>
       </c>
       <c r="D6" t="s">
-        <v>6</v>
-      </c>
-      <c r="E6" t="s">
-        <v>47</v>
-      </c>
-      <c r="F6" t="s">
-        <v>104</v>
+        <v>84</v>
       </c>
       <c r="G6" t="s">
         <v>14</v>
@@ -1017,16 +970,10 @@
         <v>7</v>
       </c>
       <c r="C7" t="s">
-        <v>65</v>
+        <v>91</v>
       </c>
       <c r="D7" t="s">
-        <v>110</v>
-      </c>
-      <c r="E7" t="s">
-        <v>47</v>
-      </c>
-      <c r="F7" t="s">
-        <v>104</v>
+        <v>84</v>
       </c>
       <c r="G7" t="s">
         <v>14</v>
@@ -1040,16 +987,10 @@
         <v>7</v>
       </c>
       <c r="C8" t="s">
-        <v>66</v>
+        <v>92</v>
       </c>
       <c r="D8" t="s">
-        <v>110</v>
-      </c>
-      <c r="E8" t="s">
-        <v>47</v>
-      </c>
-      <c r="F8" t="s">
-        <v>47</v>
+        <v>84</v>
       </c>
       <c r="G8" t="s">
         <v>14</v>
@@ -1063,16 +1004,10 @@
         <v>7</v>
       </c>
       <c r="C9" t="s">
-        <v>67</v>
+        <v>93</v>
       </c>
       <c r="D9" t="s">
-        <v>110</v>
-      </c>
-      <c r="E9" t="s">
-        <v>47</v>
-      </c>
-      <c r="F9" t="s">
-        <v>47</v>
+        <v>84</v>
       </c>
       <c r="G9" t="s">
         <v>14</v>
@@ -1086,16 +1021,10 @@
         <v>7</v>
       </c>
       <c r="C10" t="s">
-        <v>68</v>
+        <v>94</v>
       </c>
       <c r="D10" t="s">
-        <v>110</v>
-      </c>
-      <c r="E10" t="s">
-        <v>47</v>
-      </c>
-      <c r="F10" t="s">
-        <v>47</v>
+        <v>84</v>
       </c>
       <c r="G10" t="s">
         <v>14</v>
@@ -1109,16 +1038,10 @@
         <v>7</v>
       </c>
       <c r="C11" t="s">
-        <v>69</v>
+        <v>95</v>
       </c>
       <c r="D11" t="s">
-        <v>110</v>
-      </c>
-      <c r="E11" t="s">
-        <v>47</v>
-      </c>
-      <c r="F11" t="s">
-        <v>47</v>
+        <v>84</v>
       </c>
       <c r="G11" t="s">
         <v>14</v>
@@ -1132,16 +1055,10 @@
         <v>7</v>
       </c>
       <c r="C12" t="s">
-        <v>70</v>
+        <v>109</v>
       </c>
       <c r="D12" t="s">
-        <v>110</v>
-      </c>
-      <c r="E12" t="s">
-        <v>104</v>
-      </c>
-      <c r="F12" t="s">
-        <v>104</v>
+        <v>84</v>
       </c>
       <c r="G12" t="s">
         <v>14</v>
@@ -1152,19 +1069,19 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>7</v>
+        <v>85</v>
       </c>
       <c r="C13" t="s">
-        <v>71</v>
+        <v>110</v>
       </c>
       <c r="D13" t="s">
-        <v>110</v>
+        <v>6</v>
       </c>
       <c r="E13" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="F13" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="G13" t="s">
         <v>14</v>
@@ -1175,19 +1092,13 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>7</v>
+        <v>85</v>
       </c>
       <c r="C14" t="s">
-        <v>72</v>
+        <v>96</v>
       </c>
       <c r="D14" t="s">
-        <v>110</v>
-      </c>
-      <c r="E14" t="s">
-        <v>104</v>
-      </c>
-      <c r="F14" t="s">
-        <v>104</v>
+        <v>84</v>
       </c>
       <c r="G14" t="s">
         <v>14</v>
@@ -1198,19 +1109,13 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>7</v>
+        <v>85</v>
       </c>
       <c r="C15" t="s">
-        <v>73</v>
+        <v>97</v>
       </c>
       <c r="D15" t="s">
-        <v>110</v>
-      </c>
-      <c r="E15" t="s">
-        <v>104</v>
-      </c>
-      <c r="F15" t="s">
-        <v>47</v>
+        <v>84</v>
       </c>
       <c r="G15" t="s">
         <v>14</v>
@@ -1221,183 +1126,132 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>7</v>
+        <v>85</v>
       </c>
       <c r="C16" t="s">
-        <v>74</v>
+        <v>98</v>
       </c>
       <c r="D16" t="s">
-        <v>110</v>
-      </c>
-      <c r="E16" t="s">
-        <v>104</v>
-      </c>
-      <c r="F16" t="s">
-        <v>104</v>
+        <v>84</v>
       </c>
       <c r="G16" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>7</v>
+        <v>85</v>
       </c>
       <c r="C17" t="s">
-        <v>75</v>
+        <v>99</v>
       </c>
       <c r="D17" t="s">
-        <v>110</v>
-      </c>
-      <c r="E17" t="s">
-        <v>47</v>
-      </c>
-      <c r="F17" t="s">
-        <v>47</v>
+        <v>84</v>
       </c>
       <c r="G17" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>7</v>
+        <v>85</v>
       </c>
       <c r="C18" t="s">
-        <v>76</v>
+        <v>100</v>
       </c>
       <c r="D18" t="s">
-        <v>110</v>
-      </c>
-      <c r="E18" t="s">
-        <v>47</v>
-      </c>
-      <c r="F18" t="s">
-        <v>104</v>
+        <v>84</v>
       </c>
       <c r="G18" t="s">
         <v>14</v>
       </c>
-      <c r="H18" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>7</v>
+        <v>85</v>
       </c>
       <c r="C19" t="s">
-        <v>77</v>
+        <v>101</v>
       </c>
       <c r="D19" t="s">
-        <v>110</v>
-      </c>
-      <c r="E19" t="s">
-        <v>47</v>
-      </c>
-      <c r="F19" t="s">
-        <v>47</v>
+        <v>84</v>
       </c>
       <c r="G19" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>7</v>
+        <v>85</v>
       </c>
       <c r="C20" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="D20" t="s">
-        <v>110</v>
-      </c>
-      <c r="E20" t="s">
-        <v>47</v>
-      </c>
-      <c r="F20" t="s">
-        <v>47</v>
+        <v>84</v>
       </c>
       <c r="G20" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>7</v>
+        <v>85</v>
       </c>
       <c r="C21" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="D21" t="s">
-        <v>110</v>
-      </c>
-      <c r="E21" t="s">
-        <v>104</v>
-      </c>
-      <c r="F21" t="s">
-        <v>104</v>
+        <v>84</v>
       </c>
       <c r="G21" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>7</v>
+        <v>85</v>
       </c>
       <c r="C22" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="D22" t="s">
-        <v>110</v>
-      </c>
-      <c r="E22" t="s">
-        <v>104</v>
-      </c>
-      <c r="F22" t="s">
-        <v>47</v>
+        <v>84</v>
       </c>
       <c r="G22" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>7</v>
+        <v>85</v>
       </c>
       <c r="C23" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="D23" t="s">
-        <v>110</v>
-      </c>
-      <c r="E23" t="s">
-        <v>104</v>
-      </c>
-      <c r="F23" t="s">
-        <v>47</v>
+        <v>84</v>
       </c>
       <c r="G23" t="s">
         <v>14</v>
@@ -1413,8 +1267,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1422,7 +1276,7 @@
     <col min="1" max="1" width="21.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="32.42578125" customWidth="1"/>
     <col min="3" max="3" width="18.7109375" customWidth="1"/>
-    <col min="4" max="4" width="27.7109375" customWidth="1"/>
+    <col min="4" max="4" width="47.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="85.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1434,69 +1288,69 @@
         <v>5</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>59</v>
+        <v>48</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>46</v>
+        <v>111</v>
       </c>
       <c r="B2" t="s">
         <v>111</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="D2" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="E2" s="19" t="s">
-        <v>113</v>
+      <c r="E2" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C4" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C5" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C6" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C7" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C8" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1"/>
+    <hyperlink ref="A2" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId2"/>
@@ -1508,7 +1362,7 @@
   <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1529,28 +1383,40 @@
       <c r="A2" t="s">
         <v>9</v>
       </c>
+      <c r="B2" t="s">
+        <v>107</v>
+      </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>10</v>
       </c>
       <c r="B3" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>12</v>
       </c>
+      <c r="B4" t="s">
+        <v>107</v>
+      </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>13</v>
       </c>
+      <c r="B5" t="s">
+        <v>107</v>
+      </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>14</v>
+      </c>
+      <c r="B6" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -1558,37 +1424,55 @@
         <v>15</v>
       </c>
       <c r="B7" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>16</v>
       </c>
+      <c r="B8" t="s">
+        <v>107</v>
+      </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>17</v>
       </c>
+      <c r="B9" t="s">
+        <v>107</v>
+      </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>18</v>
       </c>
+      <c r="B10" t="s">
+        <v>107</v>
+      </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>19</v>
       </c>
+      <c r="B11" t="s">
+        <v>107</v>
+      </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>20</v>
       </c>
+      <c r="B12" t="s">
+        <v>107</v>
+      </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>21</v>
+      </c>
+      <c r="B13" t="s">
+        <v>107</v>
       </c>
     </row>
   </sheetData>
@@ -1619,321 +1503,321 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
-      <c r="H1" s="7"/>
-      <c r="I1" s="7"/>
-      <c r="J1" s="7"/>
-      <c r="K1" s="7"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
+      <c r="J1" s="6"/>
+      <c r="K1" s="6"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="12"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="12"/>
-      <c r="H2" s="12"/>
-      <c r="I2" s="12"/>
-      <c r="J2" s="7"/>
-      <c r="K2" s="7"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="11"/>
+      <c r="H2" s="11"/>
+      <c r="I2" s="11"/>
+      <c r="J2" s="6"/>
+      <c r="K2" s="6"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="10">
+      <c r="A3" s="9">
         <v>255</v>
       </c>
-      <c r="B3" s="10">
+      <c r="B3" s="9">
         <v>500</v>
       </c>
-      <c r="C3" s="10"/>
-      <c r="D3" s="10"/>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7"/>
-      <c r="G3" s="7"/>
-      <c r="H3" s="7"/>
-      <c r="I3" s="7"/>
-      <c r="J3" s="7"/>
-      <c r="K3" s="7"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="6"/>
+      <c r="I3" s="6"/>
+      <c r="J3" s="6"/>
+      <c r="K3" s="6"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="13" t="s">
+      <c r="A4" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="B4" s="10"/>
-      <c r="C4" s="10"/>
-      <c r="D4" s="10"/>
-      <c r="E4" s="7"/>
-      <c r="F4" s="7"/>
-      <c r="G4" s="7"/>
-      <c r="H4" s="7"/>
-      <c r="I4" s="7"/>
-      <c r="J4" s="7"/>
-      <c r="K4" s="7"/>
+      <c r="B4" s="9"/>
+      <c r="C4" s="9"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="6"/>
+      <c r="I4" s="6"/>
+      <c r="J4" s="6"/>
+      <c r="K4" s="6"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="14" t="s">
+      <c r="A5" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="B5" s="14" t="s">
+      <c r="B5" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="C5" s="14" t="s">
+      <c r="C5" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="D5" s="14" t="s">
+      <c r="D5" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="E5" s="12"/>
-      <c r="F5" s="7"/>
-      <c r="G5" s="12"/>
-      <c r="H5" s="12"/>
-      <c r="I5" s="12"/>
-      <c r="J5" s="12"/>
-      <c r="K5" s="7"/>
+      <c r="E5" s="11"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="11"/>
+      <c r="H5" s="11"/>
+      <c r="I5" s="11"/>
+      <c r="J5" s="11"/>
+      <c r="K5" s="6"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="10"/>
-      <c r="B6" s="10"/>
-      <c r="C6" s="10" t="s">
+      <c r="A6" s="9"/>
+      <c r="B6" s="9"/>
+      <c r="C6" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="D6" s="10" t="s">
+      <c r="D6" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="E6" s="7"/>
-      <c r="F6" s="7"/>
-      <c r="G6" s="7"/>
-      <c r="H6" s="7"/>
-      <c r="I6" s="7"/>
-      <c r="J6" s="7"/>
-      <c r="K6" s="7"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="6"/>
+      <c r="I6" s="6"/>
+      <c r="J6" s="6"/>
+      <c r="K6" s="6"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="13" t="s">
+      <c r="A7" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="B7" s="10"/>
-      <c r="C7" s="10"/>
-      <c r="D7" s="10"/>
-      <c r="E7" s="7"/>
-      <c r="F7" s="7"/>
-      <c r="G7" s="7"/>
-      <c r="H7" s="7"/>
-      <c r="I7" s="7"/>
-      <c r="J7" s="7"/>
-      <c r="K7" s="7"/>
+      <c r="B7" s="9"/>
+      <c r="C7" s="9"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="6"/>
+      <c r="H7" s="6"/>
+      <c r="I7" s="6"/>
+      <c r="J7" s="6"/>
+      <c r="K7" s="6"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="14" t="s">
+      <c r="A8" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="B8" s="10"/>
-      <c r="C8" s="10"/>
-      <c r="D8" s="10"/>
-      <c r="E8" s="7"/>
-      <c r="F8" s="7"/>
-      <c r="G8" s="7"/>
-      <c r="H8" s="7"/>
-      <c r="I8" s="7"/>
-      <c r="J8" s="7"/>
-      <c r="K8" s="7"/>
+      <c r="B8" s="9"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="6"/>
+      <c r="I8" s="6"/>
+      <c r="J8" s="6"/>
+      <c r="K8" s="6"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="B9" s="10"/>
-      <c r="C9" s="10"/>
-      <c r="D9" s="10"/>
-      <c r="E9" s="7"/>
-      <c r="F9" s="7"/>
-      <c r="G9" s="7"/>
-      <c r="H9" s="7"/>
-      <c r="I9" s="7"/>
-      <c r="J9" s="7"/>
-      <c r="K9" s="7"/>
+      <c r="A9" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="B9" s="9"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="6"/>
+      <c r="I9" s="6"/>
+      <c r="J9" s="6"/>
+      <c r="K9" s="6"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="10"/>
-      <c r="B10" s="10"/>
-      <c r="C10" s="10"/>
-      <c r="D10" s="10"/>
-      <c r="E10" s="7"/>
-      <c r="F10" s="7"/>
-      <c r="G10" s="7"/>
-      <c r="H10" s="7"/>
-      <c r="I10" s="7"/>
-      <c r="J10" s="7"/>
-      <c r="K10" s="7"/>
+      <c r="A10" s="9"/>
+      <c r="B10" s="9"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="6"/>
+      <c r="J10" s="6"/>
+      <c r="K10" s="6"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="13" t="s">
+      <c r="A11" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="B11" s="10"/>
-      <c r="C11" s="10"/>
-      <c r="D11" s="10"/>
-      <c r="E11" s="7"/>
-      <c r="F11" s="7"/>
-      <c r="G11" s="7"/>
-      <c r="H11" s="7"/>
-      <c r="I11" s="7"/>
-      <c r="J11" s="7"/>
-      <c r="K11" s="7"/>
+      <c r="B11" s="9"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="6"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="6"/>
+      <c r="I11" s="6"/>
+      <c r="J11" s="6"/>
+      <c r="K11" s="6"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="14"/>
-      <c r="B12" s="14" t="s">
+      <c r="A12" s="13"/>
+      <c r="B12" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="C12" s="14" t="s">
+      <c r="C12" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="D12" s="14" t="s">
+      <c r="D12" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="E12" s="14" t="s">
+      <c r="E12" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="F12" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="G12" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="H12" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="I12" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="J12" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="K12" s="13" t="s">
         <v>78</v>
       </c>
-      <c r="F12" s="14" t="s">
+    </row>
+    <row r="13" spans="1:11" s="5" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="B13" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="C13" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="D13" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="E13" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="F13" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="G13" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="H13" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="I13" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="J13" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="K13" s="15" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" s="5" customFormat="1" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="B14" s="15"/>
+      <c r="C14" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="D14" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="E14" s="16" t="s">
+        <v>68</v>
+      </c>
+      <c r="F14" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="G14" s="16" t="s">
+        <v>72</v>
+      </c>
+      <c r="H14" s="16" t="s">
+        <v>74</v>
+      </c>
+      <c r="I14" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="J14" s="16" t="s">
         <v>79</v>
       </c>
-      <c r="G12" s="14" t="s">
+      <c r="K14" s="16" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" s="5" customFormat="1" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="14" t="s">
+        <v>83</v>
+      </c>
+      <c r="B15" s="15"/>
+      <c r="C15" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="D15" s="17" t="s">
+        <v>67</v>
+      </c>
+      <c r="E15" s="17" t="s">
+        <v>69</v>
+      </c>
+      <c r="F15" s="17" t="s">
+        <v>71</v>
+      </c>
+      <c r="G15" s="17" t="s">
+        <v>73</v>
+      </c>
+      <c r="H15" s="17" t="s">
+        <v>75</v>
+      </c>
+      <c r="I15" s="17" t="s">
+        <v>77</v>
+      </c>
+      <c r="J15" s="17" t="s">
         <v>80</v>
       </c>
-      <c r="H12" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="I12" s="14" t="s">
+      <c r="K15" s="17" t="s">
         <v>82</v>
       </c>
-      <c r="J12" s="14" t="s">
-        <v>83</v>
-      </c>
-      <c r="K12" s="14" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" s="6" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="15" t="s">
-        <v>38</v>
-      </c>
-      <c r="B13" s="16" t="s">
-        <v>41</v>
-      </c>
-      <c r="C13" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="D13" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="E13" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="F13" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="G13" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="H13" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="I13" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="J13" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="K13" s="16" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" s="6" customFormat="1" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="15" t="s">
-        <v>39</v>
-      </c>
-      <c r="B14" s="16"/>
-      <c r="C14" s="16" t="s">
-        <v>84</v>
-      </c>
-      <c r="D14" s="17" t="s">
-        <v>85</v>
-      </c>
-      <c r="E14" s="17" t="s">
-        <v>88</v>
-      </c>
-      <c r="F14" s="17" t="s">
-        <v>90</v>
-      </c>
-      <c r="G14" s="17" t="s">
-        <v>92</v>
-      </c>
-      <c r="H14" s="17" t="s">
-        <v>94</v>
-      </c>
-      <c r="I14" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="J14" s="17" t="s">
-        <v>99</v>
-      </c>
-      <c r="K14" s="17" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" s="6" customFormat="1" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="15" t="s">
-        <v>103</v>
-      </c>
-      <c r="B15" s="16"/>
-      <c r="C15" s="18" t="s">
-        <v>86</v>
-      </c>
-      <c r="D15" s="18" t="s">
-        <v>87</v>
-      </c>
-      <c r="E15" s="18" t="s">
-        <v>89</v>
-      </c>
-      <c r="F15" s="18" t="s">
-        <v>91</v>
-      </c>
-      <c r="G15" s="18" t="s">
-        <v>93</v>
-      </c>
-      <c r="H15" s="18" t="s">
-        <v>95</v>
-      </c>
-      <c r="I15" s="18" t="s">
-        <v>97</v>
-      </c>
-      <c r="J15" s="18" t="s">
-        <v>100</v>
-      </c>
-      <c r="K15" s="18" t="s">
-        <v>102</v>
-      </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="13" t="s">
+      <c r="A16" s="12" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" s="10" t="s">
+      <c r="A17" s="9" t="s">
         <v>43</v>
       </c>
     </row>

</xml_diff>